<commit_message>
Dodanie kolejnych rozwiązań do zestawienia
</commit_message>
<xml_diff>
--- a/zestawienie.xlsx
+++ b/zestawienie.xlsx
@@ -11,12 +11,12 @@
     <sheet name="b" sheetId="2" r:id="rId2"/>
     <sheet name="c" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t>Nazwa rozwiązania</t>
   </si>
@@ -93,31 +93,123 @@
     <t>Outsorcing finansowy i księgowy</t>
   </si>
   <si>
-    <t>Wsprawcie z rekrutacją pracowników</t>
-  </si>
-  <si>
-    <t>CloudSocket Small Medium Enterprise (SME)</t>
-  </si>
-  <si>
     <t>Cloud Socket</t>
   </si>
   <si>
-    <t>https://site.cloudsocket.eu/sme</t>
-  </si>
-  <si>
-    <t>https://site.cloudsocket.eu/bpm-expert</t>
+    <t>Wsprarcie z rekrutacją pracowników</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>CloudSocket</t>
+  </si>
+  <si>
+    <t>https://site.cloudsocket.eu/architecture</t>
+  </si>
+  <si>
+    <t>Środowisko przeznaczone do modelowania i uruchamiania procesów biznesowych</t>
+  </si>
+  <si>
+    <t>Pomoc przy tworzeniu pakietów procesów biznesowych</t>
+  </si>
+  <si>
+    <t>Sklep BPaaS Marketplace</t>
+  </si>
+  <si>
+    <t>Środowisko przeznaczone do wdrażania (deploy'owania) procesów biznesowych w chmurze</t>
+  </si>
+  <si>
+    <t>Możliwość zarządzania instancjami BPaaS</t>
+  </si>
+  <si>
+    <t>Możliwość analizy procesów biznesowych</t>
+  </si>
+  <si>
+    <t>Finance Planning and Analysis as a Stack</t>
+  </si>
+  <si>
+    <t>Capgemini</t>
+  </si>
+  <si>
+    <t>https://www.capgemini.com/pl-pl/service/business-services/business-process-as-a-service-bpaas/finance-planning-and-analysis-as-a-stack/</t>
+  </si>
+  <si>
+    <t>Francja</t>
+  </si>
+  <si>
+    <t>Możliwość generowania dashboard'ów dotyczących procesów</t>
+  </si>
+  <si>
+    <t>Możliwość integracji z wieloma rozwiązaniami służacymi do pozyskania danych tj.: MS SQL Server, Pivotal. SAS</t>
+  </si>
+  <si>
+    <t>Możliwość korzystania z wielu rozwiązań służacych do wizualizacji danycj tj.: Tableau, QlikView</t>
+  </si>
+  <si>
+    <t>Możliwość zarządzania procesami biznesowymi</t>
+  </si>
+  <si>
+    <t>Finance-as-a-Stack on SAP S/4HANA</t>
+  </si>
+  <si>
+    <t>https://www.capgemini.com/pl-pl/service/business-services/business-process-as-a-service-bpaas/finance-as-a-stack-on-sap-s4hana/</t>
+  </si>
+  <si>
+    <t>Migracja obecnych rozwiązań do SAP S/4HANA</t>
+  </si>
+  <si>
+    <t>Uproszczone modelowanie procesów biznesowych</t>
+  </si>
+  <si>
+    <t>Możliwość analizy procesów biznesowych w dowolnym czasie i pod względem dowolnego wymiaru</t>
+  </si>
+  <si>
+    <t>Zepewnione spójne dane we wszystkich systemach</t>
+  </si>
+  <si>
+    <t>Avaloq</t>
+  </si>
+  <si>
+    <t>Szwajcaria</t>
+  </si>
+  <si>
+    <t>BPaaS</t>
+  </si>
+  <si>
+    <t>https://www.avaloq.com/en/bpaas</t>
+  </si>
+  <si>
+    <t>Automatyzacja procesów biznesowych zapewniona dzięki zastosowaniu Zrobotyzowanej Automatyzacji Procesów (Robotic Process Automation)</t>
+  </si>
+  <si>
+    <t>Automatyzacja działań zapewniona przez zastosowane rozwiązanie chmurowe</t>
+  </si>
+  <si>
+    <t>Zapewnione wspracie techniczne specjalistów od bankowości oraz od oprogramowania (24/7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zapewnione bezpieczeństwo danych </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -161,7 +253,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,6 +263,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -238,52 +336,95 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -588,204 +729,410 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="130.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="86.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="131.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="13" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="9" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="14" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="9" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="16" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="9" t="s">
+      <c r="A6" s="8"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="9" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="9" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="9" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="17" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="2" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="17" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="2" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="2" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="17" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="2" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="17" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="2" t="s">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" t="s">
-        <v>29</v>
+      <c r="E16" s="16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="23"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="23"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="23"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="24"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="29"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="29"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="29"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="16" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="24">
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="D16:D22"/>
+    <mergeCell ref="C16:C22"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="D23:D27"/>
     <mergeCell ref="B2:B9"/>
     <mergeCell ref="C2:C9"/>
     <mergeCell ref="D2:D9"/>
@@ -795,8 +1142,11 @@
     <mergeCell ref="C10:C15"/>
     <mergeCell ref="D10:D15"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C16" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Dodanie zestawienia rozwiązań w macierzy (podpunkt b)
</commit_message>
<xml_diff>
--- a/zestawienie.xlsx
+++ b/zestawienie.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="316" documentId="11_B46013A2E6724C7C1FAE3036E06B812AFD45C388" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{C9E17F11-C636-478E-A42F-C6B2A1B4B4CC}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="a" sheetId="1" r:id="rId1"/>
-    <sheet name="b" sheetId="2" r:id="rId2"/>
+    <sheet name="b" sheetId="4" r:id="rId2"/>
     <sheet name="c" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="94">
   <si>
     <t>Nazwa rozwiązania</t>
   </si>
@@ -190,18 +191,142 @@
   </si>
   <si>
     <t xml:space="preserve">Zapewnione bezpieczeństwo danych </t>
+  </si>
+  <si>
+    <t>dyPas</t>
+  </si>
+  <si>
+    <t>Expertel S.A.</t>
+  </si>
+  <si>
+    <t>https://www.proceedit.com/solutions/products</t>
+  </si>
+  <si>
+    <t>Zaawansowane programowanie warunków oraz działania platformy</t>
+  </si>
+  <si>
+    <t>Wbudowane gotowe połączenia do zewnętrznych źródeł (bazy danych, webserwisy, API itp.)</t>
+  </si>
+  <si>
+    <t>Narzędzia integracji z dowolnymi innymi aplikacji bez potrzeby programowania połączenia</t>
+  </si>
+  <si>
+    <t>Dostosowywalne środowisko</t>
+  </si>
+  <si>
+    <t>Model jednego procesu - tylko jedna klasa produktu</t>
+  </si>
+  <si>
+    <t>Zarządzanie bez pisania kodu w zakresienie wprowadzania</t>
+  </si>
+  <si>
+    <t>Cognizant</t>
+  </si>
+  <si>
+    <t>LifeAdmin Core</t>
+  </si>
+  <si>
+    <t>https://www.cognizant.com/lifeadmincore</t>
+  </si>
+  <si>
+    <t>cleaHRsky</t>
+  </si>
+  <si>
+    <t>NGA Human Resources</t>
+  </si>
+  <si>
+    <t>https://www.ngahr.com/cleahrsky</t>
+  </si>
+  <si>
+    <t>Wielka Brytania</t>
+  </si>
+  <si>
+    <t>Dodatkowe integrowalne zasoby</t>
+  </si>
+  <si>
+    <t>Integracja z zewnętrznymi serwisami</t>
+  </si>
+  <si>
+    <t>Zarządzanie bez pisania kodu w zakresie wprowadzania</t>
+  </si>
+  <si>
+    <t>Payroll</t>
+  </si>
+  <si>
+    <t>Nastawienie na proces rekrutacyjny pracowników</t>
+  </si>
+  <si>
+    <t>Wprowadzenie w przeciągu 100 dni</t>
+  </si>
+  <si>
+    <t>Szybkie rozpoczęcie</t>
+  </si>
+  <si>
+    <t>Dodatkowe materiały do nauki narzędzia</t>
+  </si>
+  <si>
+    <t>Zarządzanie listą płac</t>
+  </si>
+  <si>
+    <t>Service center</t>
+  </si>
+  <si>
+    <t>Integracja z zewnętrznymi serwisami/aplikacjami</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BPaaS </t>
+  </si>
+  <si>
+    <t>Zaawansowane wsparcie techniczne</t>
+  </si>
+  <si>
+    <t>LifeAdminCore</t>
+  </si>
+  <si>
+    <t>CleaHRsky</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>ü</t>
+  </si>
+  <si>
+    <t>capgemini</t>
+  </si>
+  <si>
+    <t>Nazwa firmy</t>
+  </si>
+  <si>
+    <t>Nazwa Rozwiązania</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -252,8 +377,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -272,8 +418,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -333,98 +503,220 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -434,12 +726,80 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF66"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="pole tekstowe 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EE2EE56-D248-4A82-881F-3FB6FBE0419D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8458200" y="3176587"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pl-PL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -485,7 +845,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -518,9 +878,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -553,6 +930,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -728,411 +1122,597 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56:C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="130.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="70.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="131.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="15" t="s">
+      <c r="A3" s="20"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="14" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="16" t="s">
+      <c r="A5" s="20"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="14" t="s">
+      <c r="A6" s="20"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="14" t="s">
+      <c r="A7" s="20"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="14" t="s">
+      <c r="A8" s="20"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="14" t="s">
+      <c r="A9" s="21"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="17" t="s">
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="17" t="s">
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="17" t="s">
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="17" t="s">
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="18" t="s">
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="19" t="s">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="16" t="s">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="16" t="s">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="16" t="s">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="16" t="s">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="16" t="s">
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E23" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="21" t="s">
+      <c r="A24" s="27"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="20" t="s">
+      <c r="A25" s="27"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="20" t="s">
+      <c r="A26" s="27"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="24"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="20" t="s">
+      <c r="A27" s="28"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="28" t="s">
+      <c r="D28" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="20" t="s">
+      <c r="A29" s="34"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="8" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="20" t="s">
+      <c r="A30" s="34"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="29"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="20" t="s">
+      <c r="A31" s="34"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E32" s="16" t="s">
+      <c r="E32" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="16" t="s">
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="16" t="s">
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="4" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="16" t="s">
+      <c r="A35" s="15"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="4" t="s">
         <v>57</v>
       </c>
     </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" s="44" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="41"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="45" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="41"/>
+      <c r="B38" s="42"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="41"/>
+      <c r="B39" s="42"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="45" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="41"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="45" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="41"/>
+      <c r="B41" s="42"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="45" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="39" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="37"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="37"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="37"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C46" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="36"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="36"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="36"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="36"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="35"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="36">
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="D46:D50"/>
+    <mergeCell ref="C46:C50"/>
+    <mergeCell ref="B46:B50"/>
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="D23:D27"/>
     <mergeCell ref="D28:D31"/>
     <mergeCell ref="C28:C31"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="A28:A31"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="D16:D22"/>
-    <mergeCell ref="C16:C22"/>
-    <mergeCell ref="B16:B22"/>
-    <mergeCell ref="A16:A22"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="D23:D27"/>
+    <mergeCell ref="B36:B41"/>
+    <mergeCell ref="C36:C41"/>
+    <mergeCell ref="D36:D41"/>
+    <mergeCell ref="A36:A41"/>
     <mergeCell ref="B2:B9"/>
     <mergeCell ref="C2:C9"/>
     <mergeCell ref="D2:D9"/>
@@ -1141,29 +1721,348 @@
     <mergeCell ref="B10:B15"/>
     <mergeCell ref="C10:C15"/>
     <mergeCell ref="D10:D15"/>
+    <mergeCell ref="D16:D22"/>
+    <mergeCell ref="C16:C22"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="A16:A22"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C16" r:id="rId1"/>
+    <hyperlink ref="C16" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{18E885FB-8CCA-45CA-BB9C-6AC2D630D746}"/>
+    <hyperlink ref="C10" r:id="rId3" xr:uid="{21D3DFDB-80DD-4F12-8D1B-E1308B67C5B7}"/>
+    <hyperlink ref="C23" r:id="rId4" xr:uid="{E3283C12-F3BF-4106-BB4D-E60EDC33CC4D}"/>
+    <hyperlink ref="C28" r:id="rId5" xr:uid="{7CAB91C2-4B1F-4D62-A73B-EBEC24568C6A}"/>
+    <hyperlink ref="C32" r:id="rId6" xr:uid="{D943A6FF-1BDC-4DA6-AFBA-09E8DCAA77EA}"/>
+    <hyperlink ref="C36" r:id="rId7" xr:uid="{E5EBE1B8-AAB7-42D1-9BE5-DBF3518FF155}"/>
+    <hyperlink ref="C46" r:id="rId8" xr:uid="{916F007D-1503-4CB1-8757-533BE3A87FB5}"/>
+    <hyperlink ref="C42" r:id="rId9" xr:uid="{57CB3F52-AB71-405C-B5C6-CFB082734354}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A88DBB9-DC45-4E27-896C-9E27F7BC5F28}">
+  <dimension ref="B1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20:F21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="46.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="57" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="58" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1" s="58" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="58" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="56" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="56" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="K3" s="54" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="I4" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="J4" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="K4" s="54" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="I5" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="J5" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="K5" s="53" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="I6" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="J6" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="K6" s="54" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="G7" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="J7" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="K7" s="54" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="H8" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="I8" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="K8" s="53" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="I9" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="J9" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="K9" s="53" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E10" s="48"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>